<commit_message>
Add in final energies for TS
</commit_message>
<xml_diff>
--- a/ncnpt_dft_energies.xlsx
+++ b/ncnpt_dft_energies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mary.vanvleet/Documents/research/collaborations/platinum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DBF5780-6E3F-214E-9689-D79DB11FAAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287D97D0-653F-ED43-A045-E4823071AD19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1060" windowWidth="27240" windowHeight="16440" xr2:uid="{6C48D67E-3D20-5246-9891-6C3C05B3CB18}"/>
+    <workbookView xWindow="-38400" yWindow="-7180" windowWidth="38400" windowHeight="21600" xr2:uid="{6C48D67E-3D20-5246-9891-6C3C05B3CB18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="92">
   <si>
     <t>au2kcalmol</t>
   </si>
@@ -129,36 +129,21 @@
     <t>TS_NCNPtMePh_NCNPt_PhMe.xyz:TS_NCNPtMePh_NCNPt_PhMe;</t>
   </si>
   <si>
-    <t>[4'/5']</t>
-  </si>
-  <si>
     <t>TS_NCNPtPhMe_NCNPt_PhMe.xyz:TS_NCNPtPhMe_NCNPt_PhMe;</t>
   </si>
   <si>
-    <t>[3'/5']</t>
-  </si>
-  <si>
     <t>TS_Ph-NCNPtMe_NCNPtMePh;</t>
   </si>
   <si>
-    <t>[4'/7']</t>
-  </si>
-  <si>
     <t>TS_NCNPtMePh_NCNPtPhMe_interconversion;</t>
   </si>
   <si>
-    <t>[3'/4']</t>
-  </si>
-  <si>
     <t>TS_NCNPtMePh_rotatePh;</t>
   </si>
   <si>
     <t>phenyl rotation in 4'</t>
   </si>
   <si>
-    <t>TS_Me-</t>
-  </si>
-  <si>
     <t>TS_NCNPtPhMe_rotatePh;</t>
   </si>
   <si>
@@ -174,9 +159,6 @@
     <t>NCNPtMePh -&gt; NCNPt + PhMe</t>
   </si>
   <si>
-    <t>old value</t>
-  </si>
-  <si>
     <t>Pathway 2: 3' -&gt; 5'</t>
   </si>
   <si>
@@ -310,6 +292,27 @@
   </si>
   <si>
     <t>Energy (a.u.)</t>
+  </si>
+  <si>
+    <t>TS_Me-NCNPtPh_NCNPtPhMe;</t>
+  </si>
+  <si>
+    <t>phenyl rotation in 3'</t>
+  </si>
+  <si>
+    <t>TS [4'/5']</t>
+  </si>
+  <si>
+    <t>TS [3'/5']</t>
+  </si>
+  <si>
+    <t>TS [4'/7']</t>
+  </si>
+  <si>
+    <t>TS [3'/4']</t>
+  </si>
+  <si>
+    <t>TS [3'/6']</t>
   </si>
 </sst>
 </file>
@@ -694,7 +697,7 @@
   <dimension ref="A1:O71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -846,16 +849,16 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -1271,12 +1274,12 @@
         <v>11</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
@@ -1312,12 +1315,12 @@
         <v>11</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
@@ -1353,12 +1356,12 @@
         <v>11</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>34</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
@@ -1394,12 +1397,12 @@
         <v>11</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
         <v>4</v>
@@ -1435,41 +1438,105 @@
         <v>11</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>39</v>
+        <v>85</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" t="s">
+        <v>8</v>
       </c>
       <c r="G17">
-        <v>-1125.4598725999999</v>
-      </c>
-      <c r="O17" s="2"/>
+        <v>-1125.45990637</v>
+      </c>
+      <c r="H17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17">
+        <v>-1124.9819399999999</v>
+      </c>
+      <c r="L17" t="s">
+        <v>11</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
+        <v>8</v>
       </c>
       <c r="G18">
-        <v>-1125.4464287599999</v>
-      </c>
-      <c r="O18" s="2"/>
+        <v>-1125.4464429899999</v>
+      </c>
+      <c r="H18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" t="s">
+        <v>8</v>
+      </c>
+      <c r="K18">
+        <v>-1124.9673720000001</v>
+      </c>
+      <c r="L18" t="s">
+        <v>11</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="H20" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G22">
         <f>G9+G10-G5</f>
@@ -1487,23 +1554,18 @@
         <f>K22*au2kcalmol</f>
         <v>-49.310949092876022</v>
       </c>
-      <c r="N22" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O22" s="1">
-        <f>-(3.2+41.5)</f>
-        <v>-44.7</v>
-      </c>
+      <c r="N22" s="2"/>
+      <c r="O22" s="1"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="O23" s="1"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="G24">
         <f>G9+G10-G7</f>
@@ -1521,23 +1583,18 @@
         <f>K24*au2kcalmol</f>
         <v>-47.700759795349668</v>
       </c>
-      <c r="N24" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O24" s="1">
-        <f>-41.5</f>
-        <v>-41.5</v>
-      </c>
+      <c r="N24" s="2"/>
+      <c r="O24" s="1"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="O25" s="1"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G26">
         <f>G3-G7</f>
@@ -1555,22 +1612,18 @@
         <f>K26*au2kcalmol</f>
         <v>-32.638650011089531</v>
       </c>
-      <c r="N26" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O26" s="1">
-        <v>-32.299999999999997</v>
-      </c>
+      <c r="N26" s="2"/>
+      <c r="O26" s="1"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="O27" s="1"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G28">
         <f>G11-G5</f>
@@ -1588,13 +1641,8 @@
         <f>K28*au2kcalmol</f>
         <v>-31.366688317427641</v>
       </c>
-      <c r="N28" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O28" s="1">
-        <f>-29.1-3.2</f>
-        <v>-32.300000000000004</v>
-      </c>
+      <c r="N28" s="2"/>
+      <c r="O28" s="1"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
@@ -1606,10 +1654,10 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="O30" s="1"/>
     </row>
@@ -1618,10 +1666,10 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G32">
         <f>G12-G5</f>
@@ -1639,23 +1687,18 @@
         <f>K32*au2kcalmol</f>
         <v>10.500115944733734</v>
       </c>
-      <c r="N32" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O32" s="1">
-        <f>12.9-3.2</f>
-        <v>9.6999999999999993</v>
-      </c>
+      <c r="N32" s="2"/>
+      <c r="O32" s="1"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="O33" s="1"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="G34">
         <f>G13-G7</f>
@@ -1673,38 +1716,39 @@
         <f>K34*au2kcalmol</f>
         <v>12.372604200353246</v>
       </c>
-      <c r="N34" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="O34" s="1">
-        <v>13.5</v>
-      </c>
+      <c r="N34" s="2"/>
+      <c r="O34" s="1"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G36">
         <f>G17-G7</f>
-        <v>8.2384800000454561E-3</v>
+        <v>8.2047099999726925E-3</v>
       </c>
       <c r="H36" s="1">
         <f>G36*au2kcalmol</f>
-        <v>5.1697242101956435</v>
-      </c>
-      <c r="O36">
-        <v>4.8</v>
+        <v>5.1485332153818542</v>
+      </c>
+      <c r="K36">
+        <f>K17-K7</f>
+        <v>5.8290000001761655E-3</v>
+      </c>
+      <c r="L36" s="1">
+        <f>K36*au2kcalmol</f>
+        <v>3.6577526949115455</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G38">
         <f>G14-G5</f>
@@ -1722,17 +1766,13 @@
         <f>K38*au2kcalmol</f>
         <v>11.063619447899816</v>
       </c>
-      <c r="O38">
-        <f>15.5-3.2</f>
-        <v>12.3</v>
-      </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G40">
         <f>G15-G7</f>
@@ -1750,16 +1790,13 @@
         <f>K40*au2kcalmol</f>
         <v>17.395817499642956</v>
       </c>
-      <c r="O40">
-        <v>15.6</v>
-      </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G42">
         <f>G16-G5</f>
@@ -1780,31 +1817,39 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G44">
         <f>G18-G7</f>
-        <v>2.1682320000081745E-2</v>
+        <v>2.1668090000048323E-2</v>
       </c>
       <c r="H44" s="1">
         <f>G44*au2kcalmol</f>
-        <v>13.605861109939376</v>
+        <v>13.596931650174533</v>
+      </c>
+      <c r="K44">
+        <f>K18-K7</f>
+        <v>2.0397000000002663E-2</v>
+      </c>
+      <c r="L44" s="1">
+        <f>K44*au2kcalmol</f>
+        <v>12.799310639194671</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="H46" s="1"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>68</v>
+      <c r="A49" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="K51">
         <f>K5-K7</f>
@@ -1817,7 +1862,7 @@
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="K53">
         <f>K9+K10-K7</f>
@@ -1830,7 +1875,7 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="K55">
         <f>K3-K7</f>
@@ -1843,7 +1888,7 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="K57">
         <f>K11-K7</f>
@@ -1856,18 +1901,18 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="K61">
         <f>K13-K7</f>
@@ -1880,10 +1925,10 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="K63">
         <f>K12-K7</f>
@@ -1899,10 +1944,10 @@
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="K65">
         <f>K14-K7</f>
@@ -1915,18 +1960,26 @@
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
+      </c>
+      <c r="K67">
+        <f>K15-K7</f>
+        <v>2.772200000003977E-2</v>
+      </c>
+      <c r="L67" s="1">
+        <f>K67*au2kcalmol</f>
+        <v>17.395817499642956</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="K69">
         <f>K16-K7</f>
@@ -1943,10 +1996,18 @@
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
+      </c>
+      <c r="K71">
+        <f>K18-K7</f>
+        <v>2.0397000000002663E-2</v>
+      </c>
+      <c r="L71" s="1">
+        <f>K71*au2kcalmol</f>
+        <v>12.799310639194671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>